<commit_message>
change numPresses to 8, fix run alternation of hands
</commit_message>
<xml_diff>
--- a/subject list.xlsx
+++ b/subject list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Experiments\Yonatan\auditory-motor-fMRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACA591C-806C-4BD9-AE01-52C52F9C4BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B500664-B2B2-4466-A6C4-EBE840756E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
   <si>
     <t>subject number</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>7 presses, only one localizer from each kind, both called motor</t>
+  </si>
+  <si>
+    <t>8 presses</t>
   </si>
 </sst>
 </file>
@@ -384,15 +387,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -457,6 +460,9 @@
       <c r="A4">
         <v>103</v>
       </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
@@ -464,6 +470,9 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>104</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
clean up git on run computer
</commit_message>
<xml_diff>
--- a/subject list.xlsx
+++ b/subject list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Experiments\Yonatan\auditory-motor-fMRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B500664-B2B2-4466-A6C4-EBE840756E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78A7508-D875-4A33-8AE6-229DA03895A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1164" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
   <si>
     <t>subject number</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>8 presses</t>
+  </si>
+  <si>
+    <t>Eyal</t>
+  </si>
+  <si>
+    <t>Ben shachar</t>
   </si>
 </sst>
 </file>
@@ -388,7 +394,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,8 +466,17 @@
       <c r="A4">
         <v>103</v>
       </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
       <c r="D4" t="s">
         <v>13</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45057</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
add subject 103 - inbal gur arye
</commit_message>
<xml_diff>
--- a/subject list.xlsx
+++ b/subject list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Experiments\Yonatan\auditory-motor-fMRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78A7508-D875-4A33-8AE6-229DA03895A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAA8DDF-F47A-471D-8FA4-71432D6155B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1164" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4920" yWindow="3468" windowWidth="17280" windowHeight="8892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
   <si>
     <t>subject number</t>
   </si>
@@ -66,13 +66,22 @@
     <t>7 presses, only one localizer from each kind, both called motor</t>
   </si>
   <si>
-    <t>8 presses</t>
-  </si>
-  <si>
     <t>Eyal</t>
   </si>
   <si>
     <t>Ben shachar</t>
+  </si>
+  <si>
+    <t>inbal</t>
+  </si>
+  <si>
+    <t>gur-arye</t>
+  </si>
+  <si>
+    <t>8 presses, data under 104</t>
+  </si>
+  <si>
+    <t>8 presses, data un,der 103, first experimental run is bad, first auditory localizer also</t>
   </si>
 </sst>
 </file>
@@ -394,7 +403,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,13 +476,13 @@
         <v>103</v>
       </c>
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1">
         <v>45057</v>
@@ -486,8 +495,17 @@
       <c r="A5">
         <v>104</v>
       </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="E5" s="1">
+        <v>45063</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
add subjects 109-110 (need to rename to 108-109)
</commit_message>
<xml_diff>
--- a/subject list.xlsx
+++ b/subject list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Experiments\Yonatan\auditory-motor-fMRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAA8DDF-F47A-471D-8FA4-71432D6155B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA26AF11-ABF7-4A3B-8899-160462E14C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="3468" windowWidth="17280" windowHeight="8892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
   <si>
     <t>subject number</t>
   </si>
@@ -82,6 +82,33 @@
   </si>
   <si>
     <t>8 presses, data un,der 103, first experimental run is bad, first auditory localizer also</t>
+  </si>
+  <si>
+    <t>ran</t>
+  </si>
+  <si>
+    <t>pulwermacher</t>
+  </si>
+  <si>
+    <t>avigail</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roni </t>
+  </si>
+  <si>
+    <t>cegla</t>
+  </si>
+  <si>
+    <t>3.7.23</t>
+  </si>
+  <si>
+    <t>yana</t>
+  </si>
+  <si>
+    <t>meistelman</t>
   </si>
 </sst>
 </file>
@@ -403,13 +430,14 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5546875" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -515,6 +543,15 @@
       <c r="A6">
         <v>105</v>
       </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45068</v>
+      </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
@@ -523,6 +560,12 @@
       <c r="A7">
         <v>106</v>
       </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45070</v>
+      </c>
       <c r="F7" t="s">
         <v>11</v>
       </c>
@@ -531,6 +574,9 @@
       <c r="A8">
         <v>107</v>
       </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
@@ -539,6 +585,15 @@
       <c r="A9">
         <v>108</v>
       </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
       <c r="F9" t="s">
         <v>11</v>
       </c>
@@ -546,6 +601,15 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
add subjects 111-112 (need to rename)
</commit_message>
<xml_diff>
--- a/subject list.xlsx
+++ b/subject list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Experiments\Yonatan\auditory-motor-fMRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958C518E-F8AE-4C8B-A055-269469FBBDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902B4DF1-FF0D-4A95-8E1F-83C05FD51284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>subject number</t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>meistelman</t>
+  </si>
+  <si>
+    <t>omri</t>
+  </si>
+  <si>
+    <t>4.7.23</t>
+  </si>
+  <si>
+    <t>punaro</t>
+  </si>
+  <si>
+    <t>nataliya</t>
+  </si>
+  <si>
+    <t>lukashov</t>
   </si>
 </sst>
 </file>
@@ -430,7 +445,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,6 +634,15 @@
       <c r="A11">
         <v>110</v>
       </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
       <c r="F11" t="s">
         <v>11</v>
       </c>
@@ -626,6 +650,15 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>

</xml_diff>